<commit_message>
Tweaked axes on linear fit check graph.
</commit_message>
<xml_diff>
--- a/ThermosFlaskModel.xlsx
+++ b/ThermosFlaskModel.xlsx
@@ -144,7 +144,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="hh:mm:ss"/>
@@ -154,7 +154,6 @@
     <numFmt numFmtId="170" formatCode="0.00"/>
     <numFmt numFmtId="171" formatCode="0.0"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
-    <numFmt numFmtId="173" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -595,20 +594,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>RunOne!$P$3:$P$6</c:f>
@@ -972,11 +957,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="35656813"/>
-        <c:axId val="68910199"/>
+        <c:axId val="34655633"/>
+        <c:axId val="35957590"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="35656813"/>
+        <c:axId val="34655633"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,12 +1017,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68910199"/>
+        <c:crossAx val="35957590"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68910199"/>
+        <c:axId val="35957590"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1087,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35656813"/>
+        <c:crossAx val="34655633"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1717,11 +1702,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="51047142"/>
-        <c:axId val="87685454"/>
+        <c:axId val="5810586"/>
+        <c:axId val="62189246"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="51047142"/>
+        <c:axId val="5810586"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70000"/>
@@ -1779,12 +1764,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87685454"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="62189246"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87685454"/>
+        <c:axId val="62189246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1849,7 +1834,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51047142"/>
+        <c:crossAx val="5810586"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2005,20 +1990,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>RunTwo!$P$3:$P$8</c:f>
@@ -2394,11 +2365,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="36292475"/>
-        <c:axId val="33531277"/>
+        <c:axId val="79386438"/>
+        <c:axId val="11949924"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36292475"/>
+        <c:axId val="79386438"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2454,12 +2425,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33531277"/>
+        <c:crossAx val="11949924"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33531277"/>
+        <c:axId val="11949924"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,7 +2495,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36292475"/>
+        <c:crossAx val="79386438"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3151,11 +3122,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="23473231"/>
-        <c:axId val="65238240"/>
+        <c:axId val="11488609"/>
+        <c:axId val="73942446"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23473231"/>
+        <c:axId val="11488609"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="67500"/>
@@ -3213,12 +3184,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65238240"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="73942446"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65238240"/>
+        <c:axId val="73942446"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3283,7 +3254,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23473231"/>
+        <c:crossAx val="11488609"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3439,20 +3410,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>RunThree!$P$3:$P$8</c:f>
@@ -3816,11 +3773,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34396206"/>
-        <c:axId val="3689088"/>
+        <c:axId val="34737742"/>
+        <c:axId val="63084641"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34396206"/>
+        <c:axId val="34737742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3876,12 +3833,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3689088"/>
+        <c:crossAx val="63084641"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3689088"/>
+        <c:axId val="63084641"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3946,7 +3903,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34396206"/>
+        <c:crossAx val="34737742"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4561,11 +4518,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48183070"/>
-        <c:axId val="45427968"/>
+        <c:axId val="61713039"/>
+        <c:axId val="26410087"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48183070"/>
+        <c:axId val="61713039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="77500"/>
@@ -4623,12 +4580,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45427968"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="26410087"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45427968"/>
+        <c:axId val="26410087"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4693,7 +4650,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48183070"/>
+        <c:crossAx val="61713039"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4881,20 +4838,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="004586"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="exp"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="1"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>BarnyRunNewStopperOne!$P$3:$P$19</c:f>
@@ -5336,11 +5279,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86870534"/>
-        <c:axId val="12630789"/>
+        <c:axId val="8819624"/>
+        <c:axId val="87582706"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86870534"/>
+        <c:axId val="8819624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5396,12 +5339,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12630789"/>
+        <c:crossAx val="87582706"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="12630789"/>
+        <c:axId val="87582706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5466,7 +5409,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86870534"/>
+        <c:crossAx val="8819624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6067,7 +6010,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarnyRunNewStopperOne!$S$57:$S$57</c:f>
+              <c:f>BarnyRunNewStopperOne!$S$57</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6159,15 +6102,15 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="45414188"/>
-        <c:axId val="59185309"/>
+        <c:axId val="44993457"/>
+        <c:axId val="23328255"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45414188"/>
+        <c:axId val="44993457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="75000"/>
-          <c:min val="67500"/>
+          <c:max val="65000"/>
+          <c:min val="55000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -6221,12 +6164,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59185309"/>
+        <c:crossAx val="23328255"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59185309"/>
+        <c:axId val="23328255"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6291,7 +6234,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45414188"/>
+        <c:crossAx val="44993457"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6382,7 +6325,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarnyRunNewStopperOne!$K$71:$K$71</c:f>
+              <c:f>BarnyRunNewStopperOne!$K$71</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6695,7 +6638,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarnyRunNewStopperOne!$K$72:$K$72</c:f>
+              <c:f>BarnyRunNewStopperOne!$K$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7008,7 +6951,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarnyRunNewStopperOne!$K$73:$K$73</c:f>
+              <c:f>BarnyRunNewStopperOne!$K$73</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7321,7 +7264,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarnyRunNewStopperOne!$K$74:$K$74</c:f>
+              <c:f>BarnyRunNewStopperOne!$K$74</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7629,11 +7572,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84713161"/>
-        <c:axId val="50713874"/>
+        <c:axId val="84472920"/>
+        <c:axId val="61665704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84713161"/>
+        <c:axId val="84472920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140000"/>
@@ -7691,12 +7634,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50713874"/>
+        <c:crossAx val="61665704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50713874"/>
+        <c:axId val="61665704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7761,7 +7704,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84713161"/>
+        <c:crossAx val="84472920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8106,8 +8049,8 @@
   </sheetPr>
   <dimension ref="B1:S62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P41" activeCellId="0" sqref="P41"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8568,7 +8511,7 @@
       </c>
       <c r="Q41" s="0" t="n">
         <f aca="false">C$23*EXP(-P41/I2)</f>
-        <v>51.9269231125672</v>
+        <v>51.9269231125671</v>
       </c>
       <c r="R41" s="0" t="n">
         <f aca="false">P41-P42</f>
@@ -8881,8 +8824,8 @@
   </sheetPr>
   <dimension ref="B1:S62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L51" activeCellId="0" sqref="L51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9477,11 +9420,11 @@
       </c>
       <c r="Q43" s="0" t="n">
         <f aca="false">C$23*EXP(-P43/I$2)</f>
-        <v>48.0524635872227</v>
+        <v>48.0524635872226</v>
       </c>
       <c r="R43" s="0" t="n">
         <f aca="false">P43-P42</f>
-        <v>3600</v>
+        <v>3600.00000000001</v>
       </c>
       <c r="S43" s="0" t="n">
         <f aca="false">R43*F44+E41</f>
@@ -9728,8 +9671,8 @@
   </sheetPr>
   <dimension ref="B1:S62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q51" activeCellId="0" sqref="Q51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10210,7 +10153,7 @@
       </c>
       <c r="Q41" s="0" t="n">
         <f aca="false">C$23*EXP(-P41/I$2)</f>
-        <v>51.7360011011415</v>
+        <v>51.7360011011416</v>
       </c>
       <c r="R41" s="0" t="n">
         <f aca="false">P41-P42</f>
@@ -10242,7 +10185,7 @@
       </c>
       <c r="Q42" s="0" t="n">
         <f aca="false">C$23*EXP(-P42/I$2)</f>
-        <v>50</v>
+        <v>50.0000000000001</v>
       </c>
       <c r="R42" s="0" t="n">
         <f aca="false">P42-P42</f>
@@ -10272,7 +10215,7 @@
       </c>
       <c r="Q43" s="0" t="n">
         <f aca="false">C$23*EXP(-P43/I$2)</f>
-        <v>48.3222504018549</v>
+        <v>48.322250401855</v>
       </c>
       <c r="R43" s="0" t="n">
         <f aca="false">P43-P42</f>
@@ -10523,8 +10466,8 @@
   </sheetPr>
   <dimension ref="B1:S74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M59" activeCellId="0" sqref="M59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I61" activeCellId="0" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10724,7 +10667,7 @@
       </c>
       <c r="L6" s="17" t="n">
         <f aca="false">K6^2</f>
-        <v>2.83387213918727E-007</v>
+        <v>2.8338721391873E-007</v>
       </c>
       <c r="M6" s="17"/>
       <c r="P6" s="15" t="n">
@@ -11687,7 +11630,7 @@
       </c>
       <c r="Q60" s="0" t="n">
         <f aca="false">C$31*EXP(-P60/K$2)</f>
-        <v>47.9501632268104</v>
+        <v>47.9501632268105</v>
       </c>
       <c r="R60" s="0" t="n">
         <f aca="false">P60-P59</f>

</xml_diff>

<commit_message>
Titied up differentials on measurements.
</commit_message>
<xml_diff>
--- a/ThermosFlaskModel.xlsx
+++ b/ThermosFlaskModel.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="29">
   <si>
     <t xml:space="preserve">Time</t>
   </si>
@@ -125,7 +125,13 @@
     <t xml:space="preserve">Meas. Differentials</t>
   </si>
   <si>
-    <t xml:space="preserve">(K/s)</t>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(℃/s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
   </si>
   <si>
     <t xml:space="preserve">Run One (SJH)</t>
@@ -297,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -406,11 +412,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -957,11 +971,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34655633"/>
-        <c:axId val="35957590"/>
+        <c:axId val="82825195"/>
+        <c:axId val="19961081"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34655633"/>
+        <c:axId val="82825195"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,12 +1031,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35957590"/>
+        <c:crossAx val="19961081"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="35957590"/>
+        <c:axId val="19961081"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,7 +1101,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34655633"/>
+        <c:crossAx val="82825195"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1702,11 +1716,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="5810586"/>
-        <c:axId val="62189246"/>
+        <c:axId val="37621505"/>
+        <c:axId val="91943158"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5810586"/>
+        <c:axId val="37621505"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70000"/>
@@ -1764,12 +1778,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62189246"/>
+        <c:crossAx val="91943158"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62189246"/>
+        <c:axId val="91943158"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,7 +1848,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5810586"/>
+        <c:crossAx val="37621505"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2365,11 +2379,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="79386438"/>
-        <c:axId val="11949924"/>
+        <c:axId val="18284552"/>
+        <c:axId val="9095373"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79386438"/>
+        <c:axId val="18284552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,12 +2439,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11949924"/>
+        <c:crossAx val="9095373"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11949924"/>
+        <c:axId val="9095373"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,7 +2509,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79386438"/>
+        <c:crossAx val="18284552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3122,11 +3136,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="11488609"/>
-        <c:axId val="73942446"/>
+        <c:axId val="49531147"/>
+        <c:axId val="13729076"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11488609"/>
+        <c:axId val="49531147"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="67500"/>
@@ -3184,12 +3198,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73942446"/>
+        <c:crossAx val="13729076"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73942446"/>
+        <c:axId val="13729076"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3254,7 +3268,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11488609"/>
+        <c:crossAx val="49531147"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3773,11 +3787,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34737742"/>
-        <c:axId val="63084641"/>
+        <c:axId val="1890746"/>
+        <c:axId val="72545791"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34737742"/>
+        <c:axId val="1890746"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3833,12 +3847,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63084641"/>
+        <c:crossAx val="72545791"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63084641"/>
+        <c:axId val="72545791"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3903,7 +3917,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34737742"/>
+        <c:crossAx val="1890746"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4518,11 +4532,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61713039"/>
-        <c:axId val="26410087"/>
+        <c:axId val="8711831"/>
+        <c:axId val="19309246"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61713039"/>
+        <c:axId val="8711831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="77500"/>
@@ -4580,12 +4594,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26410087"/>
+        <c:crossAx val="19309246"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="26410087"/>
+        <c:axId val="19309246"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4650,7 +4664,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61713039"/>
+        <c:crossAx val="8711831"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5279,11 +5293,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="8819624"/>
-        <c:axId val="87582706"/>
+        <c:axId val="12887040"/>
+        <c:axId val="19603494"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="8819624"/>
+        <c:axId val="12887040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5339,12 +5353,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87582706"/>
+        <c:crossAx val="19603494"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87582706"/>
+        <c:axId val="19603494"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5409,7 +5423,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8819624"/>
+        <c:crossAx val="12887040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6102,11 +6116,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44993457"/>
-        <c:axId val="23328255"/>
+        <c:axId val="55651993"/>
+        <c:axId val="75047830"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44993457"/>
+        <c:axId val="55651993"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="65000"/>
@@ -6164,12 +6178,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23328255"/>
+        <c:crossAx val="75047830"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="23328255"/>
+        <c:axId val="75047830"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6234,7 +6248,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44993457"/>
+        <c:crossAx val="55651993"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7572,11 +7586,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84472920"/>
-        <c:axId val="61665704"/>
+        <c:axId val="73878851"/>
+        <c:axId val="75137730"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84472920"/>
+        <c:axId val="73878851"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140000"/>
@@ -7634,12 +7648,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61665704"/>
+        <c:crossAx val="75137730"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61665704"/>
+        <c:axId val="75137730"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7704,7 +7718,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84472920"/>
+        <c:crossAx val="73878851"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7958,7 +7972,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>778320</xdr:colOff>
+      <xdr:colOff>673560</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
@@ -7982,13 +7996,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>650880</xdr:colOff>
+      <xdr:colOff>546120</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>61920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>624240</xdr:colOff>
+      <xdr:colOff>519480</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
@@ -8012,13 +8026,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>571320</xdr:colOff>
+      <xdr:colOff>466560</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>544680</xdr:colOff>
+      <xdr:colOff>439920</xdr:colOff>
       <xdr:row>88</xdr:row>
       <xdr:rowOff>93240</xdr:rowOff>
     </xdr:to>
@@ -10466,14 +10480,14 @@
   </sheetPr>
   <dimension ref="B1:S74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I61" activeCellId="0" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="12.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="12.65"/>
   </cols>
   <sheetData>
@@ -10487,11 +10501,14 @@
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>2</v>
@@ -10519,8 +10536,11 @@
       <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="27" t="s">
-        <v>22</v>
+      <c r="F2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="K2" s="9" t="n">
         <f aca="false">1/0.000011628</f>
@@ -10547,12 +10567,16 @@
       <c r="D3" s="13" t="n">
         <v>0</v>
       </c>
-      <c r="E3" s="22" t="n">
+      <c r="E3" s="19" t="n">
         <v>69.9</v>
       </c>
-      <c r="F3" s="28" t="n">
+      <c r="F3" s="27" t="n">
         <f aca="false">(E3-E4)/(D3-D4)</f>
         <v>-0.000574712643347866</v>
+      </c>
+      <c r="G3" s="28" t="n">
+        <f aca="false">F3*I$57*I$59</f>
+        <v>-3.86206896329766</v>
       </c>
       <c r="P3" s="15" t="n">
         <f aca="false">D3+F$66</f>
@@ -10575,12 +10599,16 @@
         <f aca="false">C4*24*60*60</f>
         <v>1740.000001</v>
       </c>
-      <c r="E4" s="22" t="n">
+      <c r="E4" s="19" t="n">
         <v>68.9</v>
       </c>
-      <c r="F4" s="28" t="n">
+      <c r="F4" s="27" t="n">
         <f aca="false">(E4-E5)/(D4-D5)</f>
         <v>-0.000530303030303033</v>
+      </c>
+      <c r="G4" s="28" t="n">
+        <f aca="false">F4*I$57*I$59</f>
+        <v>-3.56363636363638</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>10</v>
@@ -10606,12 +10634,16 @@
         <f aca="false">C5*24*60*60</f>
         <v>3060.000001</v>
       </c>
-      <c r="E5" s="22" t="n">
+      <c r="E5" s="19" t="n">
         <v>68.2</v>
       </c>
-      <c r="F5" s="28" t="n">
+      <c r="F5" s="27" t="n">
         <f aca="false">(E5-E6)/(D5-D6)</f>
         <v>-0.000606060606060615</v>
+      </c>
+      <c r="G5" s="28" t="n">
+        <f aca="false">F5*I$57*I$59</f>
+        <v>-4.07272727272733</v>
       </c>
       <c r="J5" s="17" t="n">
         <f aca="false">Q$3*EXP(-D3/K$2)+N$2</f>
@@ -10650,12 +10682,16 @@
         <f aca="false">C6*24*60*60</f>
         <v>3720.000001</v>
       </c>
-      <c r="E6" s="22" t="n">
+      <c r="E6" s="19" t="n">
         <v>67.8</v>
       </c>
-      <c r="F6" s="28" t="n">
+      <c r="F6" s="27" t="n">
         <f aca="false">(E6-E7)/(D6-D7)</f>
         <v>-0.000645161290322582</v>
+      </c>
+      <c r="G6" s="28" t="n">
+        <f aca="false">F6*I$57*I$59</f>
+        <v>-4.33548387096775</v>
       </c>
       <c r="J6" s="17" t="n">
         <f aca="false">Q$3*EXP(-D4/K$2)+N$2</f>
@@ -10691,12 +10727,16 @@
         <f aca="false">C7*24*60*60</f>
         <v>5580.000001</v>
       </c>
-      <c r="E7" s="22" t="n">
+      <c r="E7" s="19" t="n">
         <v>66.6</v>
       </c>
-      <c r="F7" s="28" t="n">
+      <c r="F7" s="27" t="n">
         <f aca="false">(E7-E8)/(D7-D8)</f>
         <v>-0.000531914893617021</v>
+      </c>
+      <c r="G7" s="28" t="n">
+        <f aca="false">F7*I$57*I$59</f>
+        <v>-3.57446808510638</v>
       </c>
       <c r="J7" s="17" t="n">
         <f aca="false">Q$3*EXP(-D5/K$2)+N$2</f>
@@ -10732,12 +10772,16 @@
         <f aca="false">C8*24*60*60</f>
         <v>8400.000001</v>
       </c>
-      <c r="E8" s="22" t="n">
+      <c r="E8" s="19" t="n">
         <v>65.1</v>
       </c>
-      <c r="F8" s="28" t="n">
+      <c r="F8" s="27" t="n">
         <f aca="false">(E8-E9)/(D8-D9)</f>
         <v>-0.000537634408602149</v>
+      </c>
+      <c r="G8" s="28" t="n">
+        <f aca="false">F8*I$57*I$59</f>
+        <v>-3.61290322580644</v>
       </c>
       <c r="J8" s="17" t="n">
         <f aca="false">Q$3*EXP(-D6/K$2)+N$2</f>
@@ -10773,12 +10817,16 @@
         <f aca="false">C9*24*60*60</f>
         <v>12120.000001</v>
       </c>
-      <c r="E9" s="22" t="n">
+      <c r="E9" s="19" t="n">
         <v>63.1</v>
       </c>
-      <c r="F9" s="28" t="n">
+      <c r="F9" s="27" t="n">
         <f aca="false">(E9-E10)/(D9-D10)</f>
         <v>-0.00050925925925926</v>
+      </c>
+      <c r="G9" s="28" t="n">
+        <f aca="false">F9*I$57*I$59</f>
+        <v>-3.42222222222223</v>
       </c>
       <c r="J9" s="17" t="n">
         <f aca="false">Q$3*EXP(-D7/K$2)+N$2</f>
@@ -10813,12 +10861,16 @@
         <f aca="false">C10*24*60*60</f>
         <v>14280.000001</v>
       </c>
-      <c r="E10" s="22" t="n">
+      <c r="E10" s="19" t="n">
         <v>62</v>
       </c>
-      <c r="F10" s="28" t="n">
+      <c r="F10" s="27" t="n">
         <f aca="false">(E10-E11)/(D10-D11)</f>
         <v>-0.000459770114942529</v>
+      </c>
+      <c r="G10" s="28" t="n">
+        <f aca="false">F10*I$57*I$59</f>
+        <v>-3.08965517241379</v>
       </c>
       <c r="J10" s="17" t="n">
         <f aca="false">Q$3*EXP(-D8/K$2)+N$2</f>
@@ -10853,12 +10905,16 @@
         <f aca="false">C11*24*60*60</f>
         <v>17760.000001</v>
       </c>
-      <c r="E11" s="22" t="n">
+      <c r="E11" s="19" t="n">
         <v>60.4</v>
       </c>
-      <c r="F11" s="28" t="n">
+      <c r="F11" s="27" t="n">
         <f aca="false">(E11-E12)/(D11-D12)</f>
         <v>-0.000465116279069765</v>
+      </c>
+      <c r="G11" s="28" t="n">
+        <f aca="false">F11*I$57*I$59</f>
+        <v>-3.12558139534882</v>
       </c>
       <c r="J11" s="17" t="n">
         <f aca="false">Q$3*EXP(-D9/K$2)+N$2</f>
@@ -10893,12 +10949,16 @@
         <f aca="false">C12*24*60*60</f>
         <v>20340.000001</v>
       </c>
-      <c r="E12" s="22" t="n">
+      <c r="E12" s="19" t="n">
         <v>59.2</v>
       </c>
-      <c r="F12" s="28" t="n">
+      <c r="F12" s="27" t="n">
         <f aca="false">(E12-E13)/(D12-D13)</f>
         <v>-0.000396825396825397</v>
+      </c>
+      <c r="G12" s="28" t="n">
+        <f aca="false">F12*I$57*I$59</f>
+        <v>-2.66666666666667</v>
       </c>
       <c r="J12" s="17" t="n">
         <f aca="false">Q$3*EXP(-D10/K$2)+N$2</f>
@@ -10933,12 +10993,16 @@
         <f aca="false">C13*24*60*60</f>
         <v>29160.000001</v>
       </c>
-      <c r="E13" s="22" t="n">
+      <c r="E13" s="19" t="n">
         <v>55.7</v>
       </c>
-      <c r="F13" s="28" t="n">
+      <c r="F13" s="27" t="n">
         <f aca="false">(E13-E14)/(D13-D14)</f>
         <v>-0.000394736842162974</v>
+      </c>
+      <c r="G13" s="28" t="n">
+        <f aca="false">F13*I$57*I$59</f>
+        <v>-2.65263157933519</v>
       </c>
       <c r="J13" s="17" t="n">
         <f aca="false">Q$3*EXP(-D11/K$2)+N$2</f>
@@ -10973,12 +11037,16 @@
         <f aca="false">C14*24*60*60</f>
         <v>36000</v>
       </c>
-      <c r="E14" s="22" t="n">
+      <c r="E14" s="19" t="n">
         <v>53</v>
       </c>
-      <c r="F14" s="28" t="n">
+      <c r="F14" s="27" t="n">
         <f aca="false">(E14-E15)/(D14-D15)</f>
         <v>-0.000375586854371928</v>
+      </c>
+      <c r="G14" s="28" t="n">
+        <f aca="false">F14*I$57*I$59</f>
+        <v>-2.52394366137936</v>
       </c>
       <c r="J14" s="17" t="n">
         <f aca="false">Q$3*EXP(-D12/K$2)+N$2</f>
@@ -11013,12 +11081,16 @@
         <f aca="false">C15*24*60*60</f>
         <v>40260.000001</v>
       </c>
-      <c r="E15" s="22" t="n">
+      <c r="E15" s="19" t="n">
         <v>51.4</v>
       </c>
-      <c r="F15" s="28" t="n">
+      <c r="F15" s="27" t="n">
         <f aca="false">(E15-E16)/(D15-D16)</f>
         <v>-0.000361445783205109</v>
+      </c>
+      <c r="G15" s="28" t="n">
+        <f aca="false">F15*I$57*I$59</f>
+        <v>-2.42891566313833</v>
       </c>
       <c r="J15" s="17" t="n">
         <f aca="false">Q$3*EXP(-D13/K$2)+N$2</f>
@@ -11053,12 +11125,16 @@
         <f aca="false">C16*24*60*60</f>
         <v>45240</v>
       </c>
-      <c r="E16" s="22" t="n">
+      <c r="E16" s="19" t="n">
         <v>49.6</v>
       </c>
-      <c r="F16" s="28" t="n">
+      <c r="F16" s="27" t="n">
         <f aca="false">(E16-E17)/(D16-D17)</f>
         <v>-0.000340909090779958</v>
+      </c>
+      <c r="G16" s="28" t="n">
+        <f aca="false">F16*I$57*I$59</f>
+        <v>-2.29090909004132</v>
       </c>
       <c r="J16" s="17" t="n">
         <f aca="false">Q$3*EXP(-D14/K$2)+N$2</f>
@@ -11093,12 +11169,16 @@
         <f aca="false">C17*24*60*60</f>
         <v>47880.000001</v>
       </c>
-      <c r="E17" s="22" t="n">
+      <c r="E17" s="19" t="n">
         <v>48.7</v>
       </c>
-      <c r="F17" s="28" t="n">
+      <c r="F17" s="27" t="n">
         <f aca="false">(E17-E18)/(D17-D18)</f>
         <v>-0.000320512820553912</v>
+      </c>
+      <c r="G17" s="28" t="n">
+        <f aca="false">F17*I$57*I$59</f>
+        <v>-2.15384615412229</v>
       </c>
       <c r="J17" s="17" t="n">
         <f aca="false">Q$3*EXP(-D15/K$2)+N$2</f>
@@ -11133,12 +11213,16 @@
         <f aca="false">C18*24*60*60</f>
         <v>55680</v>
       </c>
-      <c r="E18" s="22" t="n">
+      <c r="E18" s="19" t="n">
         <v>46.2</v>
       </c>
-      <c r="F18" s="28" t="n">
+      <c r="F18" s="27" t="n">
         <f aca="false">(E18-E19)/(D18-D19)</f>
         <v>-0.000267072346170823</v>
+      </c>
+      <c r="G18" s="28" t="n">
+        <f aca="false">F18*I$57*I$59</f>
+        <v>-1.79472616626793</v>
       </c>
       <c r="J18" s="17" t="n">
         <f aca="false">Q$3*EXP(-D16/K$2)+N$2</f>
@@ -11173,13 +11257,11 @@
         <f aca="false">C19*24*60*60</f>
         <v>85260.000001</v>
       </c>
-      <c r="E19" s="22" t="n">
+      <c r="E19" s="19" t="n">
         <v>38.3</v>
       </c>
-      <c r="F19" s="28" t="n">
-        <f aca="false">(E19-E20)/(D19-D20)</f>
-        <v>0.000449214168420722</v>
-      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30"/>
       <c r="J19" s="17" t="n">
         <f aca="false">Q$3*EXP(-D17/K$2)+N$2</f>
         <v>48.5961577028349</v>
@@ -11774,22 +11856,22 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K71" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K72" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K73" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K74" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>